<commit_message>
Fixed more problems with Excel parsing
</commit_message>
<xml_diff>
--- a/validator/src/test/resources/samples/ColumnsOfNamedCellsAndGroupsMultipleSheets.xlsx
+++ b/validator/src/test/resources/samples/ColumnsOfNamedCellsAndGroupsMultipleSheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\copia\CACAO\validator\src\test\resources\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9706F7FA-14A8-47D0-8115-C506BDF77859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DFBCB1-9D8C-4483-BE2D-50FCB58E6208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,12 +21,12 @@
     <definedName name="Id">Plan1!$E$4</definedName>
     <definedName name="Name" localSheetId="1">Plan2!$E$3</definedName>
     <definedName name="Name">Plan1!$E$3</definedName>
-    <definedName name="ProductCode" localSheetId="1">Plan2!$C$8:$C$13</definedName>
-    <definedName name="ProductCode">Plan1!$C$8:$C$13</definedName>
-    <definedName name="ProductName" localSheetId="1">Plan2!$D$8:$D$13</definedName>
-    <definedName name="ProductName">Plan1!$D$8:$D$13</definedName>
-    <definedName name="UnityPrice" localSheetId="1">Plan2!$E$8:$E$13</definedName>
-    <definedName name="UnityPrice">Plan1!$E$8:$E$13</definedName>
+    <definedName name="ProductCode" localSheetId="1">Plan2!$C$8:$C$18</definedName>
+    <definedName name="ProductCode">Plan1!$C$8:$C$18</definedName>
+    <definedName name="ProductName" localSheetId="1">Plan2!$D$8:$D$18</definedName>
+    <definedName name="ProductName">Plan1!$D$8:$D$18</definedName>
+    <definedName name="UnityPrice" localSheetId="1">Plan2!$E$8:$E$18</definedName>
+    <definedName name="UnityPrice">Plan1!$E$8:$E$18</definedName>
     <definedName name="Year" localSheetId="1">Plan2!$E$5</definedName>
     <definedName name="Year">Plan1!$E$5</definedName>
   </definedNames>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>Name:</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Scissors</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:E13"/>
+  <dimension ref="B3:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,60 +560,112 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="s">
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E10" s="3">
         <v>800</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="3">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E14" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C12" s="2" t="s">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E16" s="3">
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C13" s="2" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E18" s="3">
         <v>300</v>
       </c>
     </row>
@@ -621,10 +676,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBFF0EB-CE9A-4FC3-AED1-BF3B7134D845}">
-  <dimension ref="B3:E13"/>
+  <dimension ref="B3:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -685,60 +740,112 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="s">
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E10" s="3">
         <v>800</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="3">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E14" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C12" s="2" t="s">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E16" s="3">
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C13" s="2" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E18" s="3">
         <v>300</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Additional field for sorting data at Dashboards according to line position
</commit_message>
<xml_diff>
--- a/validator/src/test/resources/samples/ColumnsOfNamedCellsAndGroupsMultipleSheets.xlsx
+++ b/validator/src/test/resources/samples/ColumnsOfNamedCellsAndGroupsMultipleSheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\copia\CACAO\validator\src\test\resources\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DFBCB1-9D8C-4483-BE2D-50FCB58E6208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EA7984-0E6B-4802-AD14-C592CFE515D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -21,11 +21,11 @@
     <definedName name="Id">Plan1!$E$4</definedName>
     <definedName name="Name" localSheetId="1">Plan2!$E$3</definedName>
     <definedName name="Name">Plan1!$E$3</definedName>
-    <definedName name="ProductCode" localSheetId="1">Plan2!$C$8:$C$18</definedName>
+    <definedName name="ProductCode" localSheetId="1">Plan2!$C$13:$C$23</definedName>
     <definedName name="ProductCode">Plan1!$C$8:$C$18</definedName>
-    <definedName name="ProductName" localSheetId="1">Plan2!$D$8:$D$18</definedName>
+    <definedName name="ProductName" localSheetId="1">Plan2!$D$13:$D$23</definedName>
     <definedName name="ProductName">Plan1!$D$8:$D$18</definedName>
-    <definedName name="UnityPrice" localSheetId="1">Plan2!$E$8:$E$18</definedName>
+    <definedName name="UnityPrice" localSheetId="1">Plan2!$E$13:$E$23</definedName>
     <definedName name="UnityPrice">Plan1!$E$8:$E$18</definedName>
     <definedName name="Year" localSheetId="1">Plan2!$E$5</definedName>
     <definedName name="Year">Plan1!$E$5</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>Name:</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>additional rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not included in </t>
+  </si>
+  <si>
+    <t>previous sheet.</t>
+  </si>
+  <si>
+    <t>Some intentionally</t>
   </si>
 </sst>
 </file>
@@ -210,11 +222,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -498,186 +511,6 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="3">
-        <v>300</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBFF0EB-CE9A-4FC3-AED1-BF3B7134D845}">
-  <dimension ref="B3:E18"/>
-  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
@@ -727,13 +560,13 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E8" s="3">
         <v>1000</v>
@@ -752,10 +585,10 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E10" s="3">
         <v>800</v>
@@ -774,10 +607,10 @@
         <v>35</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E12" s="3">
         <v>50</v>
@@ -793,13 +626,13 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E14" s="3">
         <v>100</v>
@@ -818,10 +651,10 @@
         <v>35</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E16" s="3">
         <v>200</v>
@@ -840,12 +673,224 @@
         <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="3">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBFF0EB-CE9A-4FC3-AED1-BF3B7134D845}">
+  <dimension ref="B3:E23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="3">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E23" s="3">
         <v>300</v>
       </c>
     </row>

</xml_diff>